<commit_message>
dodanie opcji okreslenia oreintacji etykiet na osi x
</commit_message>
<xml_diff>
--- a/pages/ma_details_files/promise.xlsx
+++ b/pages/ma_details_files/promise.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\PycharmProjects\streamlit_test_1\pages\ma_details_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C35CA9A-69FB-44D1-8996-B6DEF6B30760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D95A3FB0-3B65-4586-AB05-7DC934404307}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="26116" windowHeight="15675" xr2:uid="{37C2049F-C855-49AB-ABEF-6CD6C9A1CCEC}"/>
   </bookViews>
@@ -57,9 +57,6 @@
     <t>Dzienniczek wdzięczności 2</t>
   </si>
   <si>
-    <t>DZIENNICZEK WDZIĘCZNOŚCI</t>
-  </si>
-  <si>
     <t>Dzienniczek wdzięczności</t>
   </si>
   <si>
@@ -112,6 +109,9 @@
   </si>
   <si>
     <t>1 dziesiątka różańca</t>
+  </si>
+  <si>
+    <t>DZIENNICZEK</t>
   </si>
 </sst>
 </file>
@@ -483,7 +483,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -517,7 +517,7 @@
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -531,7 +531,7 @@
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -542,10 +542,10 @@
         <v>2022</v>
       </c>
       <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
         <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -556,10 +556,10 @@
         <v>2022</v>
       </c>
       <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
         <v>14</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -570,10 +570,10 @@
         <v>2021</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -584,10 +584,10 @@
         <v>2021</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -598,10 +598,10 @@
         <v>2021</v>
       </c>
       <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" t="s">
         <v>17</v>
-      </c>
-      <c r="D8" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -612,10 +612,10 @@
         <v>2021</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -626,10 +626,10 @@
         <v>2020</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -640,10 +640,10 @@
         <v>2020</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -654,10 +654,10 @@
         <v>2020</v>
       </c>
       <c r="C12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -668,10 +668,10 @@
         <v>2020</v>
       </c>
       <c r="C13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -682,24 +682,24 @@
         <v>2019</v>
       </c>
       <c r="C14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B15">
         <v>2019</v>
       </c>
       <c r="C15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" t="s">
         <v>24</v>
-      </c>
-      <c r="D15" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -710,10 +710,10 @@
         <v>2019</v>
       </c>
       <c r="C16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -724,10 +724,10 @@
         <v>2019</v>
       </c>
       <c r="C17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dodano raprotyz duzych liczb
</commit_message>
<xml_diff>
--- a/pages/ma_details_files/promise.xlsx
+++ b/pages/ma_details_files/promise.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\PycharmProjects\streamlit_test_1\pages\ma_details_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D95A3FB0-3B65-4586-AB05-7DC934404307}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DB2E6AD-F463-48A1-9B1A-2CC6CB4B3EF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="26116" windowHeight="15675" xr2:uid="{37C2049F-C855-49AB-ABEF-6CD6C9A1CCEC}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="30">
   <si>
     <t>MAILING Q4</t>
   </si>
@@ -112,6 +112,9 @@
   </si>
   <si>
     <t>DZIENNICZEK</t>
+  </si>
+  <si>
+    <t>Katechezy</t>
   </si>
 </sst>
 </file>
@@ -480,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65040E38-94CE-4377-BD3C-9535D34BC24E}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -730,6 +733,20 @@
         <v>12</v>
       </c>
     </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18">
+        <v>2023</v>
+      </c>
+      <c r="C18" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>